<commit_message>
generating output tables for website
</commit_message>
<xml_diff>
--- a/website/Modifications_to_NHSEstimatesSchema.xlsx
+++ b/website/Modifications_to_NHSEstimatesSchema.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18990" windowHeight="7395"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18990" windowHeight="7395" tabRatio="726" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="397">
   <si>
     <t>table_name</t>
   </si>
@@ -1220,6 +1220,9 @@
   </si>
   <si>
     <t>comments for updated database</t>
+  </si>
+  <si>
+    <t>Parsum2</t>
   </si>
 </sst>
 </file>
@@ -1592,8 +1595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2204,7 +2207,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>28</v>
+        <v>396</v>
       </c>
       <c r="B34" s="8">
         <v>5</v>
@@ -2224,7 +2227,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>28</v>
+        <v>396</v>
       </c>
       <c r="B35" s="8">
         <v>6</v>
@@ -2241,7 +2244,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>28</v>
+        <v>396</v>
       </c>
       <c r="B36" s="8">
         <v>7</v>
@@ -2258,7 +2261,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
-        <v>28</v>
+        <v>396</v>
       </c>
       <c r="B37" s="8">
         <v>8</v>
@@ -2275,7 +2278,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
-        <v>28</v>
+        <v>396</v>
       </c>
       <c r="B38" s="8">
         <v>9</v>
@@ -2292,7 +2295,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
-        <v>28</v>
+        <v>396</v>
       </c>
       <c r="B39" s="8">
         <v>10</v>
@@ -2312,7 +2315,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
-        <v>28</v>
+        <v>396</v>
       </c>
       <c r="B40" s="8">
         <v>11</v>
@@ -2329,7 +2332,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
-        <v>28</v>
+        <v>396</v>
       </c>
       <c r="B41" s="8">
         <v>12</v>
@@ -2346,7 +2349,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
-        <v>28</v>
+        <v>396</v>
       </c>
       <c r="B42" s="8">
         <v>13</v>
@@ -2922,7 +2925,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="B8:C8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3406,12 +3409,12 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:D10"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="36" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="2" max="2" width="81.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3622,8 +3625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4454,8 +4457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>